<commit_message>
Added Crypt Utils, And Other features
</commit_message>
<xml_diff>
--- a/resources/Recon_Driver_Config.xlsx
+++ b/resources/Recon_Driver_Config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Source Name</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Store_ID</t>
+  </si>
+  <si>
+    <t>Legacy_Store_File1</t>
+  </si>
+  <si>
+    <t>New_Store_DB1</t>
   </si>
 </sst>
 </file>
@@ -482,17 +488,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -502,7 +508,7 @@
     <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -510,7 +516,7 @@
     <col min="18" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -643,6 +649,71 @@
         <v>36</v>
       </c>
     </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <v>1433</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3">
+        <v>1521</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes for Source and Target Column Mappings.
</commit_message>
<xml_diff>
--- a/resources/Recon_Driver_Config.xlsx
+++ b/resources/Recon_Driver_Config.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Recon_Config" sheetId="1" r:id="rId1"/>
-    <sheet name="Config_Usage" sheetId="2" r:id="rId2"/>
+    <sheet name="Legacy_vs_New" sheetId="3" r:id="rId2"/>
+    <sheet name="Config_Usage" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Source Name</t>
   </si>
@@ -153,6 +154,27 @@
   </si>
   <si>
     <t>Cloud source and target</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Legacy_vs_New</t>
+  </si>
+  <si>
+    <t>Source_Column</t>
+  </si>
+  <si>
+    <t>Target_Column</t>
+  </si>
+  <si>
+    <t>Store_Number</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -518,164 +540,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="59.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>1433</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>1521</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -686,10 +715,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>